<commit_message>
Adding data and starting to clean
</commit_message>
<xml_diff>
--- a/Data/ManyLabs1_Data.xlsx
+++ b/Data/ManyLabs1_Data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D4CB8D-CA90-4204-8143-00EB655CCBD0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C85128FB-E37B-4F55-B302-8F29F08BEC84}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,26 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="93">
   <si>
     <t>Effect</t>
   </si>
   <si>
-    <t>ES</t>
-  </si>
-  <si>
-    <t>95% CI Lower, Upper</t>
-  </si>
-  <si>
-    <t>Median Replication ES</t>
-  </si>
-  <si>
-    <t>Replication ES</t>
-  </si>
-  <si>
-    <t>99% CI Lower, Upper</t>
-  </si>
-  <si>
     <t>Proportion &lt;0 (p&lt;.05)</t>
   </si>
   <si>
@@ -49,18 +34,6 @@
     <t>Proportion ns</t>
   </si>
   <si>
-    <t>Key statistics</t>
-  </si>
-  <si>
-    <t>df</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>p</t>
-  </si>
-  <si>
     <t>Anchoring - Babies Born</t>
   </si>
   <si>
@@ -293,6 +266,39 @@
   </si>
   <si>
     <t>t=-0.79</t>
+  </si>
+  <si>
+    <t>Replication ES.r</t>
+  </si>
+  <si>
+    <t>Median Replication ES.r</t>
+  </si>
+  <si>
+    <t>ES.o</t>
+  </si>
+  <si>
+    <t>95% CI Lower, Upper.o</t>
+  </si>
+  <si>
+    <t>99% CI Lower, Upper.r</t>
+  </si>
+  <si>
+    <t>Replication ES.r.unweighted.DNU</t>
+  </si>
+  <si>
+    <t>99% CI Lower, Upper.r.unweighted.DNU</t>
+  </si>
+  <si>
+    <t>Key statistics.r</t>
+  </si>
+  <si>
+    <t>df.r</t>
+  </si>
+  <si>
+    <t>N.r</t>
+  </si>
+  <si>
+    <t>p.r</t>
   </si>
 </sst>
 </file>
@@ -673,68 +679,68 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="38.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="K1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="L1" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="38.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
-        <v>13</v>
       </c>
       <c r="B2" s="9">
         <v>0.93</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D2" s="9">
         <v>2.4300000000000002</v>
@@ -743,13 +749,13 @@
         <v>2.6</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="G2" s="9">
         <v>2.42</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="I2" s="9">
         <v>0</v>
@@ -761,7 +767,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="M2" s="10">
         <v>5607</v>
@@ -770,18 +776,18 @@
         <v>5609</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="38.5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="39" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3">
         <v>0.93</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D3" s="3">
         <v>2</v>
@@ -790,13 +796,13 @@
         <v>2.4500000000000002</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="G3" s="3">
         <v>2.23</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="I3" s="3">
         <v>0</v>
@@ -808,7 +814,7 @@
         <v>0</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="M3" s="2">
         <v>5625</v>
@@ -817,18 +823,18 @@
         <v>5627</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="26" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B4" s="3">
         <v>0.65</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D4" s="3">
         <v>1.88</v>
@@ -837,13 +843,13 @@
         <v>1.87</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="G4" s="3">
         <v>1.96</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="I4" s="3">
         <v>0</v>
@@ -855,7 +861,7 @@
         <v>2.777777777777779E-2</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="M4" s="2">
         <v>1</v>
@@ -864,18 +870,18 @@
         <v>6292</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="26" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="39" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B5" s="3">
         <v>0.93</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D5" s="3">
         <v>1.88</v>
@@ -884,13 +890,13 @@
         <v>2.0499999999999998</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="G5" s="3">
         <v>1.79</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="I5" s="3">
         <v>0</v>
@@ -902,7 +908,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="M5" s="2">
         <v>5282</v>
@@ -911,18 +917,18 @@
         <v>5284</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="51" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B6" s="3">
         <v>0.93</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D6" s="3">
         <v>1.18</v>
@@ -931,13 +937,13 @@
         <v>1.27</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="G6" s="3">
         <v>1.17</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="I6" s="3">
         <v>0</v>
@@ -949,7 +955,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="M6" s="2">
         <v>5360</v>
@@ -958,18 +964,18 @@
         <v>5362</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="63.5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B7" s="3">
         <v>0.93</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="D7" s="3">
         <v>0.84</v>
@@ -978,13 +984,13 @@
         <v>0.79</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="G7" s="3">
         <v>0.79</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="I7" s="3">
         <v>0</v>
@@ -996,25 +1002,25 @@
         <v>5.7142857142857162E-2</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="M7" s="2"/>
       <c r="N7" s="2">
         <v>5623</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="51" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B8" s="3">
         <v>0.69</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D8" s="3">
         <v>0.61</v>
@@ -1023,13 +1029,13 @@
         <v>0.59</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="G8" s="3">
         <v>0.61</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="I8" s="3">
         <v>0</v>
@@ -1041,7 +1047,7 @@
         <v>0.16666666666666663</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="M8" s="2">
         <v>5940</v>
@@ -1050,18 +1056,18 @@
         <v>5942</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="38.5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="39" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B9" s="3">
         <v>1.1299999999999999</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D9" s="3">
         <v>0.57999999999999996</v>
@@ -1070,13 +1076,13 @@
         <v>0.62</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="G9" s="3">
         <v>0.6</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="I9" s="3">
         <v>0</v>
@@ -1088,7 +1094,7 @@
         <v>0.13888888888888884</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="M9" s="2">
         <v>1</v>
@@ -1097,18 +1103,18 @@
         <v>6271</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="76" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B10" s="3">
         <v>1.01</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="D10" s="3">
         <v>0.59</v>
@@ -1117,13 +1123,13 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="G10" s="3">
         <v>0.53</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="I10" s="3">
         <v>0</v>
@@ -1135,7 +1141,7 @@
         <v>0.2857142857142857</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="M10" s="2">
         <v>5840</v>
@@ -1144,18 +1150,18 @@
         <v>5842</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="51" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B11" s="3">
         <v>0.5</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D11" s="3">
         <v>0.5</v>
@@ -1164,13 +1170,13 @@
         <v>0.51</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="G11" s="3">
         <v>0.49</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="I11" s="3">
         <v>0</v>
@@ -1182,7 +1188,7 @@
         <v>0.33333333333333337</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="M11" s="2">
         <v>1</v>
@@ -1191,15 +1197,15 @@
         <v>5899</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="38.5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="39" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3">
@@ -1209,13 +1215,13 @@
         <v>0.31</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G12" s="3">
         <v>0.32</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="I12" s="3">
         <v>0</v>
@@ -1227,7 +1233,7 @@
         <v>0.52777777777777779</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="M12" s="2">
         <v>6323</v>
@@ -1236,18 +1242,18 @@
         <v>6325</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="38.5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="39" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B13" s="3">
         <v>0.16</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D13" s="3">
         <v>0.27</v>
@@ -1256,13 +1262,13 @@
         <v>0.27</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="G13" s="3">
         <v>0.3</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="I13" s="3">
         <v>0</v>
@@ -1274,7 +1280,7 @@
         <v>0.63888888888888884</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="M13" s="2">
         <v>1</v>
@@ -1283,18 +1289,18 @@
         <v>6276</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="26" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B14" s="3">
         <v>0.227912862495395</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D14" s="3">
         <v>0.32</v>
@@ -1303,13 +1309,13 @@
         <v>0.31</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="G14" s="3">
         <v>0.27</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="I14" s="3">
         <v>0</v>
@@ -1321,7 +1327,7 @@
         <v>0.5</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="M14" s="2">
         <v>6328</v>
@@ -1330,18 +1336,18 @@
         <v>6330</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="26" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B15" s="3">
         <v>0.86</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D15" s="3">
         <v>0.12</v>
@@ -1350,13 +1356,13 @@
         <v>0.1</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="G15" s="3">
         <v>0.13</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="I15" s="3">
         <v>2.7777777777777776E-2</v>
@@ -1368,7 +1374,7 @@
         <v>0.86111111111111116</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="M15" s="2">
         <v>6334</v>
@@ -1377,18 +1383,18 @@
         <v>6336</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="26" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B16" s="3">
         <v>0.5</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D16" s="3">
         <v>1.9E-2</v>
@@ -1397,13 +1403,13 @@
         <v>0.01</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="G16" s="3">
         <v>0.03</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="I16" s="3">
         <v>0.04</v>
@@ -1415,7 +1421,7 @@
         <v>0.96</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="M16" s="2">
         <v>4894</v>
@@ -1427,15 +1433,15 @@
         <v>0.379</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="26" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="B17" s="6">
         <v>0.8</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D17" s="6">
         <v>0</v>
@@ -1444,13 +1450,13 @@
         <v>0.01</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="G17" s="6">
         <v>-0.02</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="I17" s="6">
         <v>0</v>
@@ -1462,7 +1468,7 @@
         <v>0.97222222222222221</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="M17" s="5">
         <v>6331</v>

</xml_diff>

<commit_message>
Continuing cleaning and adding in LOOPR results
</commit_message>
<xml_diff>
--- a/Data/ManyLabs1_Data.xlsx
+++ b/Data/ManyLabs1_Data.xlsx
@@ -3,24 +3,29 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C85128FB-E37B-4F55-B302-8F29F08BEC84}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B78500F-DD0C-4155-8797-595B12405BC0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="104">
   <si>
     <t>Effect</t>
   </si>
@@ -299,6 +304,39 @@
   </si>
   <si>
     <t>p.r</t>
+  </si>
+  <si>
+    <t>testStatistic.o</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> F(1, 211) = 2.74, p = .1, partial η2=.01</t>
+  </si>
+  <si>
+    <t>No statistical test reported</t>
+  </si>
+  <si>
+    <t>t(57) = 2.65, p &lt; .05, Cohen’s d = 0.69</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> χ2(1)= 7.7, p &lt; .01</t>
+  </si>
+  <si>
+    <t>t(64) = -2.04, p &lt; .05</t>
+  </si>
+  <si>
+    <t>t(28) = 2.12, p = .043, d = 0.80</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> t(31) = -2.39, p = .023, d = .86</t>
+  </si>
+  <si>
+    <t>r = .42</t>
+  </si>
+  <si>
+    <t>t(77) = 4.42, p = 10e-5 , d = 1.01</t>
+  </si>
+  <si>
+    <t>r = .42, n = 243</t>
   </si>
 </sst>
 </file>
@@ -317,12 +355,14 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -364,7 +404,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -394,6 +434,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -677,15 +720,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="AC6" sqref="AC6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -731,8 +774,11 @@
       <c r="O1" s="5" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="P1" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
@@ -778,8 +824,11 @@
       <c r="O2" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" ht="39" x14ac:dyDescent="0.25">
+      <c r="P2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -825,8 +874,11 @@
       <c r="O3" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="P3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -872,8 +924,11 @@
       <c r="O4" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" ht="39" x14ac:dyDescent="0.25">
+      <c r="P4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -919,8 +974,11 @@
       <c r="O5" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="P5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -966,8 +1024,11 @@
       <c r="O6" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" ht="64.5" x14ac:dyDescent="0.25">
+      <c r="P6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
@@ -1011,8 +1072,11 @@
       <c r="O7" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="P7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>32</v>
       </c>
@@ -1058,8 +1122,11 @@
       <c r="O8" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" ht="39" x14ac:dyDescent="0.25">
+      <c r="P8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
@@ -1105,8 +1172,11 @@
       <c r="O9" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" ht="77.25" x14ac:dyDescent="0.25">
+      <c r="P9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>42</v>
       </c>
@@ -1152,8 +1222,11 @@
       <c r="O10" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="P10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>47</v>
       </c>
@@ -1199,8 +1272,11 @@
       <c r="O11" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" ht="39" x14ac:dyDescent="0.25">
+      <c r="P11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>52</v>
       </c>
@@ -1244,8 +1320,11 @@
       <c r="O12" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" ht="39" x14ac:dyDescent="0.25">
+      <c r="P12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>57</v>
       </c>
@@ -1291,8 +1370,11 @@
       <c r="O13" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="P13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>62</v>
       </c>
@@ -1338,8 +1420,11 @@
       <c r="O14" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="P14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>67</v>
       </c>
@@ -1385,8 +1470,11 @@
       <c r="O15" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="P15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>72</v>
       </c>
@@ -1432,8 +1520,11 @@
       <c r="O16" s="2">
         <v>0.379</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="P16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>77</v>
       </c>
@@ -1479,8 +1570,12 @@
       <c r="O17" s="5">
         <v>0.83099999999999996</v>
       </c>
+      <c r="P17" t="s">
+        <v>99</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>